<commit_message>
Refactored common PostingLabel functionality for Journey controllers to a common class
</commit_message>
<xml_diff>
--- a/src/apodeixi/knowledge_base/tests_integration/input_data/basic_posting_flows.big_rocks.explained/products.static-data.admin.a6i.xlsx
+++ b/src/apodeixi/knowledge_base/tests_integration/input_data/basic_posting_flows.big_rocks.explained/products.static-data.admin.a6i.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\knowledge_base\tests_integration\input_data\basic_posting_flows.big_rocks.explained\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E410FD-5231-4BD2-820B-9FDC0AB91E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD81C532-B0D7-4AAF-8041-D277EC1E2F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -672,7 +672,7 @@
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>